<commit_message>
fix mv comparison, update pp comparison
</commit_message>
<xml_diff>
--- a/results/comparisons/missing-values-impact/mv-10Folds.xlsx
+++ b/results/comparisons/missing-values-impact/mv-10Folds.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33020" windowHeight="16060" tabRatio="986"/>
+    <workbookView xWindow="22000" yWindow="0" windowWidth="17980" windowHeight="22200" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="Avg" sheetId="1" r:id="rId1"/>
@@ -542,6 +542,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,14 +559,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -939,7 +939,7 @@
   <dimension ref="A1:JJ64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -949,6 +949,7 @@
     <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.33203125" customWidth="1"/>
     <col min="12" max="12" width="18.5" customWidth="1"/>
     <col min="13" max="13" width="8.1640625" customWidth="1"/>
@@ -1030,7 +1031,7 @@
         <v>59</v>
       </c>
       <c r="M6" s="9"/>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="18" t="s">
         <v>69</v>
       </c>
       <c r="O6" s="2" t="s">
@@ -1076,8 +1077,8 @@
         <f t="shared" ref="N7:N55" si="0">C7-H7</f>
         <v>-2.9665699897649667E-3</v>
       </c>
-      <c r="O7" s="24">
-        <f>G7-B7</f>
+      <c r="O7" s="19">
+        <f t="shared" ref="O7:O38" si="1">G7-B7</f>
         <v>0</v>
       </c>
     </row>
@@ -1108,11 +1109,11 @@
         <v>0.213541194701385</v>
       </c>
       <c r="K8" s="11" t="str">
-        <f t="shared" ref="K8:K55" si="1">IF(C8=0,"out",IF(B8&gt;G8,"better without pp",IF(B8=G8,"same","better with pp")))</f>
+        <f t="shared" ref="K8:K55" si="2">IF(C8=0,"out",IF(B8&gt;G8,"better without pp",IF(B8=G8,"same","better with pp")))</f>
         <v>same</v>
       </c>
       <c r="L8" s="11" t="str">
-        <f t="shared" ref="L8:L55" si="2">IF(D8=0,"out",IF(C8&gt;H8,"better without pp",IF(C8=H8,"same","better with pp")))</f>
+        <f t="shared" ref="L8:L55" si="3">IF(D8=0,"out",IF(C8&gt;H8,"better without pp",IF(C8=H8,"same","better with pp")))</f>
         <v>better with pp</v>
       </c>
       <c r="M8" s="9"/>
@@ -1120,8 +1121,8 @@
         <f t="shared" si="0"/>
         <v>-3.5854013937189899E-3</v>
       </c>
-      <c r="O8" s="24">
-        <f>G8-B8</f>
+      <c r="O8" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1152,11 +1153,11 @@
         <v>0.20403064708174801</v>
       </c>
       <c r="K9" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L9" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M9" s="9"/>
@@ -1164,8 +1165,8 @@
         <f t="shared" si="0"/>
         <v>-2.637740163787039E-3</v>
       </c>
-      <c r="O9" s="24">
-        <f>G9-B9</f>
+      <c r="O9" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1196,11 +1197,11 @@
         <v>0.22293503373624901</v>
       </c>
       <c r="K10" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L10" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M10" s="9"/>
@@ -1208,8 +1209,8 @@
         <f t="shared" si="0"/>
         <v>-3.9100162944329941E-3</v>
       </c>
-      <c r="O10" s="24">
-        <f>G10-B10</f>
+      <c r="O10" s="19">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
@@ -1240,11 +1241,11 @@
         <v>0.213203716833993</v>
       </c>
       <c r="K11" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L11" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M11" s="9"/>
@@ -1252,8 +1253,8 @@
         <f t="shared" si="0"/>
         <v>2.4008749228859871E-3</v>
       </c>
-      <c r="O11" s="24">
-        <f>G11-B11</f>
+      <c r="O11" s="19">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1284,11 +1285,11 @@
         <v>0.22321380424732301</v>
       </c>
       <c r="K12" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L12" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M12" s="9"/>
@@ -1296,8 +1297,8 @@
         <f t="shared" si="0"/>
         <v>5.1824341678419206E-3</v>
       </c>
-      <c r="O12" s="24">
-        <f>G12-B12</f>
+      <c r="O12" s="19">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1328,11 +1329,11 @@
         <v>0.20932193763274501</v>
       </c>
       <c r="K13" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L13" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M13" s="9"/>
@@ -1340,8 +1341,8 @@
         <f t="shared" si="0"/>
         <v>6.3348040530808447E-4</v>
       </c>
-      <c r="O13" s="24">
-        <f>G13-B13</f>
+      <c r="O13" s="19">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1372,11 +1373,11 @@
         <v>0.217135850906649</v>
       </c>
       <c r="K14" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L14" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M14" s="9"/>
@@ -1384,8 +1385,8 @@
         <f t="shared" si="0"/>
         <v>-5.0378635543050221E-3</v>
       </c>
-      <c r="O14" s="24">
-        <f>G14-B14</f>
+      <c r="O14" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1416,11 +1417,11 @@
         <v>0.21189385797475399</v>
       </c>
       <c r="K15" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L15" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M15" s="9"/>
@@ -1428,8 +1429,8 @@
         <f t="shared" si="0"/>
         <v>2.3540609625090081E-3</v>
       </c>
-      <c r="O15" s="24">
-        <f>G15-B15</f>
+      <c r="O15" s="19">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1460,19 +1461,19 @@
         <v>0.20544171580193901</v>
       </c>
       <c r="K16" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L16" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="N16" s="12">
         <f t="shared" si="0"/>
         <v>-7.5216502611660241E-3</v>
       </c>
-      <c r="O16" s="24">
-        <f>G16-B16</f>
+      <c r="O16" s="19">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
@@ -1503,11 +1504,11 @@
         <v>0.225174734900215</v>
       </c>
       <c r="K17" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L17" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M17" s="9"/>
@@ -1515,8 +1516,8 @@
         <f t="shared" si="0"/>
         <v>7.1168180305619666E-3</v>
       </c>
-      <c r="O17" s="24">
-        <f>G17-B17</f>
+      <c r="O17" s="19">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -1547,11 +1548,11 @@
         <v>0.22463935522569001</v>
       </c>
       <c r="K18" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L18" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M18" s="9"/>
@@ -1559,8 +1560,8 @@
         <f t="shared" si="0"/>
         <v>-3.7404176542830125E-3</v>
       </c>
-      <c r="O18" s="24">
-        <f>G18-B18</f>
+      <c r="O18" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1591,19 +1592,19 @@
         <v>0.21099113098910999</v>
       </c>
       <c r="K19" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L19" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="N19" s="12">
         <f t="shared" si="0"/>
         <v>-5.3453406549709426E-3</v>
       </c>
-      <c r="O19" s="24">
-        <f>G19-B19</f>
+      <c r="O19" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1634,19 +1635,19 @@
         <v>0.219032456848157</v>
       </c>
       <c r="K20" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L20" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="N20" s="12">
         <f t="shared" si="0"/>
         <v>1.1537548727783009E-2</v>
       </c>
-      <c r="O20" s="24">
-        <f>G20-B20</f>
+      <c r="O20" s="19">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -1677,11 +1678,11 @@
         <v>0.22809304850599599</v>
       </c>
       <c r="K21" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L21" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M21" s="9"/>
@@ -1689,8 +1690,8 @@
         <f t="shared" si="0"/>
         <v>1.323510133703909E-3</v>
       </c>
-      <c r="O21" s="24">
-        <f>G21-B21</f>
+      <c r="O21" s="19">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1722,11 +1723,11 @@
       </c>
       <c r="J22"/>
       <c r="K22" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L22" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M22" s="9"/>
@@ -1734,8 +1735,8 @@
         <f t="shared" si="0"/>
         <v>-1.6615990826629456E-3</v>
       </c>
-      <c r="O22" s="24">
-        <f>G22-B22</f>
+      <c r="O22" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P22" s="7"/>
@@ -2022,11 +2023,11 @@
       </c>
       <c r="J23"/>
       <c r="K23" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L23" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M23" s="9"/>
@@ -2034,8 +2035,8 @@
         <f t="shared" si="0"/>
         <v>-5.5941719725659533E-3</v>
       </c>
-      <c r="O23" s="24">
-        <f>G23-B23</f>
+      <c r="O23" s="19">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="P23" s="7"/>
@@ -2322,11 +2323,11 @@
       </c>
       <c r="J24"/>
       <c r="K24" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L24" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M24" s="9"/>
@@ -2334,8 +2335,8 @@
         <f t="shared" si="0"/>
         <v>-4.6863885631310831E-3</v>
       </c>
-      <c r="O24" s="24">
-        <f>G24-B24</f>
+      <c r="O24" s="19">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="P24" s="7"/>
@@ -2622,11 +2623,11 @@
       </c>
       <c r="J25"/>
       <c r="K25" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L25" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M25" s="9"/>
@@ -2634,8 +2635,8 @@
         <f t="shared" si="0"/>
         <v>-5.6762785132800087E-3</v>
       </c>
-      <c r="O25" s="24">
-        <f>G25-B25</f>
+      <c r="O25" s="19">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="P25" s="7"/>
@@ -2921,11 +2922,11 @@
         <v>0.209293498008333</v>
       </c>
       <c r="K26" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L26" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M26" s="9"/>
@@ -2933,8 +2934,8 @@
         <f t="shared" si="0"/>
         <v>-5.3299543385980641E-3</v>
       </c>
-      <c r="O26" s="24">
-        <f>G26-B26</f>
+      <c r="O26" s="19">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
@@ -2966,11 +2967,11 @@
       </c>
       <c r="J27"/>
       <c r="K27" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L27" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M27" s="9"/>
@@ -2978,8 +2979,8 @@
         <f t="shared" si="0"/>
         <v>5.5902835319530109E-3</v>
       </c>
-      <c r="O27" s="24">
-        <f>G27-B27</f>
+      <c r="O27" s="19">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P27" s="7"/>
@@ -3265,11 +3266,11 @@
         <v>0.21576890734024601</v>
       </c>
       <c r="K28" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L28" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M28" s="9"/>
@@ -3277,8 +3278,8 @@
         <f t="shared" si="0"/>
         <v>-8.7704722488100018E-3</v>
       </c>
-      <c r="O28" s="24">
-        <f>G28-B28</f>
+      <c r="O28" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3309,11 +3310,11 @@
         <v>0.24615069977916701</v>
       </c>
       <c r="K29" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L29" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M29" s="9"/>
@@ -3321,8 +3322,8 @@
         <f t="shared" si="0"/>
         <v>-1.8528269317430457E-3</v>
       </c>
-      <c r="O29" s="24">
-        <f>G29-B29</f>
+      <c r="O29" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3353,11 +3354,11 @@
         <v>0.22738827788124499</v>
       </c>
       <c r="K30" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L30" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M30" s="9"/>
@@ -3365,8 +3366,8 @@
         <f t="shared" si="0"/>
         <v>-2.9019163464250042E-3</v>
       </c>
-      <c r="O30" s="24">
-        <f>G30-B30</f>
+      <c r="O30" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3397,11 +3398,11 @@
         <v>0.20360146905422299</v>
       </c>
       <c r="K31" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L31" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M31" s="9"/>
@@ -3409,8 +3410,8 @@
         <f t="shared" si="0"/>
         <v>-8.1626936603670375E-3</v>
       </c>
-      <c r="O31" s="24">
-        <f>G31-B31</f>
+      <c r="O31" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3442,11 +3443,11 @@
       </c>
       <c r="J32"/>
       <c r="K32" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L32" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M32" s="9"/>
@@ -3454,8 +3455,8 @@
         <f t="shared" si="0"/>
         <v>-2.4326020006240068E-3</v>
       </c>
-      <c r="O32" s="24">
-        <f>G32-B32</f>
+      <c r="O32" s="19">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P32" s="7"/>
@@ -3741,11 +3742,11 @@
         <v>0.21068793815717099</v>
       </c>
       <c r="K33" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L33" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M33" s="9"/>
@@ -3753,8 +3754,8 @@
         <f t="shared" si="0"/>
         <v>8.0580736067220604E-3</v>
       </c>
-      <c r="O33" s="24">
-        <f>G33-B33</f>
+      <c r="O33" s="19">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -3785,11 +3786,11 @@
         <v>0.22647030624869599</v>
       </c>
       <c r="K34" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L34" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M34" s="9"/>
@@ -3797,8 +3798,8 @@
         <f t="shared" si="0"/>
         <v>-4.5266074043480709E-3</v>
       </c>
-      <c r="O34" s="24">
-        <f>G34-B34</f>
+      <c r="O34" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3829,11 +3830,11 @@
         <v>0.22249015542664399</v>
       </c>
       <c r="K35" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L35" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M35" s="9"/>
@@ -3841,8 +3842,8 @@
         <f t="shared" si="0"/>
         <v>5.268464593778055E-3</v>
       </c>
-      <c r="O35" s="24">
-        <f>G35-B35</f>
+      <c r="O35" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3873,11 +3874,11 @@
         <v>0.19784398642263901</v>
       </c>
       <c r="K36" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L36" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M36" s="9"/>
@@ -3885,8 +3886,8 @@
         <f t="shared" si="0"/>
         <v>3.7721193005900711E-3</v>
       </c>
-      <c r="O36" s="24">
-        <f>G36-B36</f>
+      <c r="O36" s="19">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -3917,11 +3918,11 @@
         <v>0.204990733956461</v>
       </c>
       <c r="K37" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L37" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M37" s="9"/>
@@ -3929,8 +3930,8 @@
         <f t="shared" si="0"/>
         <v>-5.0492664327410619E-3</v>
       </c>
-      <c r="O37" s="24">
-        <f>G37-B37</f>
+      <c r="O37" s="19">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -3962,11 +3963,11 @@
       </c>
       <c r="J38"/>
       <c r="K38" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L38" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M38" s="9"/>
@@ -3974,8 +3975,8 @@
         <f t="shared" si="0"/>
         <v>-3.081676577498027E-3</v>
       </c>
-      <c r="O38" s="24">
-        <f>G38-B38</f>
+      <c r="O38" s="19">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
       <c r="P38" s="7"/>
@@ -4261,11 +4262,11 @@
         <v>0.19866298488822601</v>
       </c>
       <c r="K39" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L39" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M39" s="9"/>
@@ -4273,8 +4274,8 @@
         <f t="shared" si="0"/>
         <v>1.0682159615187925E-2</v>
       </c>
-      <c r="O39" s="24">
-        <f>G39-B39</f>
+      <c r="O39" s="19">
+        <f t="shared" ref="O39:O55" si="4">G39-B39</f>
         <v>1</v>
       </c>
     </row>
@@ -4305,11 +4306,11 @@
         <v>0.25447299435488202</v>
       </c>
       <c r="K40" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L40" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M40" s="9"/>
@@ -4317,8 +4318,8 @@
         <f t="shared" si="0"/>
         <v>5.3659556905168992E-3</v>
       </c>
-      <c r="O40" s="24">
-        <f>G40-B40</f>
+      <c r="O40" s="19">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4349,11 +4350,11 @@
         <v>0.23256068917703401</v>
       </c>
       <c r="K41" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L41" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M41" s="9"/>
@@ -4361,8 +4362,8 @@
         <f t="shared" si="0"/>
         <v>2.6548112067570351E-3</v>
       </c>
-      <c r="O41" s="24">
-        <f>G41-B41</f>
+      <c r="O41" s="19">
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
@@ -4393,11 +4394,11 @@
         <v>0.212326088147586</v>
       </c>
       <c r="K42" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L42" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M42" s="9"/>
@@ -4405,8 +4406,8 @@
         <f t="shared" si="0"/>
         <v>5.1244255709880226E-3</v>
       </c>
-      <c r="O42" s="24">
-        <f>G42-B42</f>
+      <c r="O42" s="19">
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
@@ -4438,11 +4439,11 @@
       </c>
       <c r="J43"/>
       <c r="K43" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L43" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M43" s="9"/>
@@ -4450,8 +4451,8 @@
         <f t="shared" si="0"/>
         <v>-4.1769986761940325E-3</v>
       </c>
-      <c r="O43" s="24">
-        <f>G43-B43</f>
+      <c r="O43" s="19">
+        <f t="shared" si="4"/>
         <v>-2</v>
       </c>
       <c r="P43" s="7"/>
@@ -4737,11 +4738,11 @@
         <v>0.224038125865894</v>
       </c>
       <c r="K44" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L44" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M44" s="13"/>
@@ -4749,8 +4750,8 @@
         <f t="shared" si="0"/>
         <v>-1.0462747630302083E-4</v>
       </c>
-      <c r="O44" s="24">
-        <f>G44-B44</f>
+      <c r="O44" s="19">
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
@@ -4781,11 +4782,11 @@
         <v>0.24106011969410901</v>
       </c>
       <c r="K45" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L45" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M45" s="9"/>
@@ -4793,8 +4794,8 @@
         <f t="shared" si="0"/>
         <v>-4.1363703708989785E-3</v>
       </c>
-      <c r="O45" s="24">
-        <f>G45-B45</f>
+      <c r="O45" s="19">
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
@@ -4825,11 +4826,11 @@
         <v>0.26713998481967199</v>
       </c>
       <c r="K46" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L46" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M46" s="9"/>
@@ -4837,8 +4838,8 @@
         <f t="shared" si="0"/>
         <v>2.0536218514060067E-3</v>
       </c>
-      <c r="O46" s="24">
-        <f>G46-B46</f>
+      <c r="O46" s="19">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -4869,11 +4870,11 @@
         <v>0.188076057301021</v>
       </c>
       <c r="K47" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better with pp</v>
       </c>
       <c r="L47" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M47" s="9"/>
@@ -4881,8 +4882,8 @@
         <f t="shared" si="0"/>
         <v>9.3527166539290052E-3</v>
       </c>
-      <c r="O47" s="24">
-        <f>G47-B47</f>
+      <c r="O47" s="19">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -4913,11 +4914,11 @@
         <v>0.27178418010571398</v>
       </c>
       <c r="K48" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L48" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M48" s="9"/>
@@ -4925,8 +4926,8 @@
         <f t="shared" si="0"/>
         <v>3.5577458765350123E-3</v>
       </c>
-      <c r="O48" s="24">
-        <f>G48-B48</f>
+      <c r="O48" s="19">
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
@@ -4957,11 +4958,11 @@
         <v>0.24029073600572101</v>
       </c>
       <c r="K49" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>better without pp</v>
       </c>
       <c r="L49" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M49" s="9"/>
@@ -4969,8 +4970,8 @@
         <f t="shared" si="0"/>
         <v>-4.9469894652509616E-3</v>
       </c>
-      <c r="O49" s="24">
-        <f>G49-B49</f>
+      <c r="O49" s="19">
+        <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
@@ -5001,11 +5002,11 @@
         <v>0.31710125026841401</v>
       </c>
       <c r="K50" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L50" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M50" s="9"/>
@@ -5013,8 +5014,8 @@
         <f t="shared" si="0"/>
         <v>2.6323715495100153E-3</v>
       </c>
-      <c r="O50" s="24">
-        <f>G50-B50</f>
+      <c r="O50" s="19">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5046,11 +5047,11 @@
       </c>
       <c r="J51"/>
       <c r="K51" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L51" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M51" s="9"/>
@@ -5058,8 +5059,8 @@
         <f t="shared" si="0"/>
         <v>8.2379984522820138E-3</v>
       </c>
-      <c r="O51" s="24">
-        <f>G51-B51</f>
+      <c r="O51" s="19">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P51" s="7"/>
@@ -5345,11 +5346,11 @@
         <v>0.23376053653777901</v>
       </c>
       <c r="K52" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L52" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M52" s="9"/>
@@ -5357,8 +5358,8 @@
         <f t="shared" si="0"/>
         <v>3.4043669319470116E-3</v>
       </c>
-      <c r="O52" s="24">
-        <f>G52-B52</f>
+      <c r="O52" s="19">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5389,11 +5390,11 @@
         <v>0.228861779799194</v>
       </c>
       <c r="K53" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L53" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better without pp</v>
       </c>
       <c r="M53" s="9"/>
@@ -5401,8 +5402,8 @@
         <f t="shared" si="0"/>
         <v>9.5502675617087363E-5</v>
       </c>
-      <c r="O53" s="24">
-        <f>G53-B53</f>
+      <c r="O53" s="19">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5433,11 +5434,11 @@
         <v>0.30558851371626899</v>
       </c>
       <c r="K54" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L54" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="M54" s="9"/>
@@ -5445,8 +5446,8 @@
         <f t="shared" si="0"/>
         <v>-6.949282465549321E-2</v>
       </c>
-      <c r="O54" s="24">
-        <f>G54-B54</f>
+      <c r="O54" s="19">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5477,19 +5478,19 @@
         <v>0.29051001831594703</v>
       </c>
       <c r="K55" s="11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>same</v>
       </c>
       <c r="L55" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>better with pp</v>
       </c>
       <c r="N55" s="12">
         <f t="shared" si="0"/>
         <v>-7.1398332940311809E-2</v>
       </c>
-      <c r="O55" s="24">
-        <f>G55-B55</f>
+      <c r="O55" s="19">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -5537,62 +5538,62 @@
     </row>
     <row r="61" spans="1:270" ht="15">
       <c r="A61" s="16"/>
-      <c r="B61" s="18" t="s">
+      <c r="B61" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="19"/>
-      <c r="D61" s="20" t="s">
+      <c r="C61" s="23"/>
+      <c r="D61" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="E61" s="19"/>
+      <c r="E61" s="23"/>
       <c r="F61" s="15"/>
     </row>
     <row r="62" spans="1:270" ht="15">
       <c r="A62" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="21">
+      <c r="B62" s="20">
         <f>COUNTIF($K$7:$K$55,$A62)</f>
         <v>21</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="21">
+      <c r="C62" s="21"/>
+      <c r="D62" s="20">
         <f>COUNTIF($L$7:$L$55,$A62)</f>
         <v>0</v>
       </c>
-      <c r="E62" s="22"/>
+      <c r="E62" s="21"/>
       <c r="F62" s="14"/>
     </row>
     <row r="63" spans="1:270" ht="15">
       <c r="A63" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="21">
-        <f t="shared" ref="B63:B64" si="3">COUNTIF($K$7:$K$55,$A63)</f>
+      <c r="B63" s="20">
+        <f t="shared" ref="B63:B64" si="5">COUNTIF($K$7:$K$55,$A63)</f>
         <v>14</v>
       </c>
-      <c r="C63" s="22"/>
-      <c r="D63" s="21">
-        <f t="shared" ref="D63:D64" si="4">COUNTIF($L$7:$L$55,$A63)</f>
+      <c r="C63" s="21"/>
+      <c r="D63" s="20">
+        <f t="shared" ref="D63:D64" si="6">COUNTIF($L$7:$L$55,$A63)</f>
         <v>27</v>
       </c>
-      <c r="E63" s="22"/>
+      <c r="E63" s="21"/>
       <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:270" ht="15">
       <c r="A64" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="21">
-        <f t="shared" si="3"/>
+      <c r="B64" s="20">
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="21">
-        <f t="shared" si="4"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="20">
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="E64" s="22"/>
+      <c r="E64" s="21"/>
       <c r="F64" s="14"/>
     </row>
   </sheetData>
@@ -5610,7 +5611,6 @@
     <mergeCell ref="D63:E63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
update figures in excel files
</commit_message>
<xml_diff>
--- a/results/comparisons/missing-values-impact/mv-10Folds.xlsx
+++ b/results/comparisons/missing-values-impact/mv-10Folds.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="986"/>
+    <workbookView xWindow="19900" yWindow="0" windowWidth="18500" windowHeight="22200" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="Avg" sheetId="1" r:id="rId1"/>
@@ -822,22 +822,22 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="327">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1197,8 +1197,344 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
+            <c:v>Rank without missing values pre-processing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Avg!$A$7:$A$55</c:f>
+              <c:strCache>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>RotationForest J48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MultiboostAB, PART</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Bagging NBTree</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bagging PART</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bagging J48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MultiboostAB NBTree</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Alternating Decision Tree</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>RotationForest RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Logistic Model Tree</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Bagging JRip</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>MultiboostAB J48</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>MultiboostAB, Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>PART</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>J48</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>DTNB</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>NBTree</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>OrdinalClassClassifier J48</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>AdaboostM1, J48</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Bagging RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>JRip</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Bagging Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>LogitBoost Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>RandomComittee RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Decision Table</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>MultiboostAB, Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Random Subspaces of RepTree</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Ridor</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>IBk</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Bagging Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Bagging RepTree</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Bagging LWL</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>IB1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Naive Bayes</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>LWL</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>MultiboostAB, RepTree</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Bagging Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>MultiboostAB, RandomTree</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>MultiboostAB DecisionStump</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Rep Tree</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>AdaboostM1, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Decision Stump</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>VFI</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Conjunctive Rule</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Decorate</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Random Tree</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Raced Incremental Logit Boost, Decision Stumps</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>OneR</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Bagging OneR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Avg!$B$7:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="49"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
             <c:v>Rank with missing values pre-processing</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1494,328 +1830,6 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>14.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>16.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Rank without missing values pre-processing</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>Avg!$A$7:$A$55</c:f>
-              <c:strCache>
-                <c:ptCount val="49"/>
-                <c:pt idx="0">
-                  <c:v>RotationForest J48</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>MultiboostAB, PART</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Bagging NBTree</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Bagging PART</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Bagging J48</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>MultiboostAB NBTree</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Alternating Decision Tree</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>RotationForest RandomTree</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Logistic Model Tree</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Bagging JRip</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>MultiboostAB J48</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>MultiboostAB, Decision Table</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>PART</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>J48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>DTNB</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>NBTree</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>OrdinalClassClassifier J48</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>AdaboostM1, J48</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Random Forest</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Bagging RandomTree</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>JRip</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>Bagging Decision Table</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>LogitBoost Decision Stump</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>RandomComittee RandomTree</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Decision Table</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>MultiboostAB, Naive Bayes</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Random Subspaces of RepTree</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Ridor</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>IBk</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Bagging Naive Bayes</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Bagging RepTree</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Bagging LWL</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>IB1</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Naive Bayes</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>LWL</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>MultiboostAB, RepTree</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Bagging Decision Stump</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>MultiboostAB, RandomTree</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>MultiboostAB DecisionStump</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Rep Tree</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>AdaboostM1, Decision Stumps</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Decision Stump</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>VFI</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Conjunctive Rule</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Decorate</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Random Tree</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Raced Incremental Logit Boost, Decision Stumps</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>OneR</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Bagging OneR</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Avg!$B$7:$B$55</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>12.0</c:v>
@@ -1847,11 +1861,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2139139416"/>
-        <c:axId val="2117826888"/>
+        <c:axId val="-2113723096"/>
+        <c:axId val="-2108674008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2139139416"/>
+        <c:axId val="-2113723096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1860,7 +1874,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2117826888"/>
+        <c:crossAx val="-2108674008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1868,7 +1882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117826888"/>
+        <c:axId val="-2108674008"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:min val="1.0"/>
@@ -1880,15 +1894,34 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2139139416"/>
+        <c:crossAx val="-2113723096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0410460991671669"/>
+          <c:y val="0.89320684537826"/>
+          <c:w val="0.691245545541793"/>
+          <c:h val="0.0996787740387466"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1907,15 +1940,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>430695</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>7363</xdr:rowOff>
+      <xdr:colOff>42333</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>151298</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>452782</xdr:colOff>
-      <xdr:row>101</xdr:row>
-      <xdr:rowOff>99392</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>59265</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>118534</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2261,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JJ64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -7065,73 +7098,73 @@
       <c r="M59" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="N59" s="23">
+      <c r="N59" s="19">
         <f>AVERAGE(N7:N55)</f>
         <v>2.9046582382137977E-3</v>
       </c>
-      <c r="O59" s="23">
+      <c r="O59" s="19">
         <f>AVERAGE(O7:O55)</f>
         <v>0.12244897959183673</v>
       </c>
     </row>
     <row r="61" spans="1:270" ht="15">
       <c r="A61" s="17"/>
-      <c r="B61" s="19" t="s">
+      <c r="B61" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="18"/>
-      <c r="D61" s="19" t="s">
+      <c r="C61" s="23"/>
+      <c r="D61" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="E61" s="18"/>
+      <c r="E61" s="23"/>
       <c r="F61" s="10"/>
     </row>
     <row r="62" spans="1:270" ht="15">
-      <c r="A62" s="20" t="s">
+      <c r="A62" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="21">
+      <c r="B62" s="20">
         <f>COUNTIF($K$7:$K$55,$A62)</f>
         <v>0</v>
       </c>
-      <c r="C62" s="22"/>
-      <c r="D62" s="21">
+      <c r="C62" s="21"/>
+      <c r="D62" s="20">
         <f>COUNTIF($L$7:$L$55,$A62)</f>
         <v>21</v>
       </c>
-      <c r="E62" s="22"/>
+      <c r="E62" s="21"/>
       <c r="F62" s="9"/>
     </row>
     <row r="63" spans="1:270" ht="15">
-      <c r="A63" s="20" t="s">
+      <c r="A63" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="21">
+      <c r="B63" s="20">
         <f t="shared" ref="B63:B64" si="5">COUNTIF($K$7:$K$55,$A63)</f>
         <v>27</v>
       </c>
-      <c r="C63" s="22"/>
-      <c r="D63" s="21">
+      <c r="C63" s="21"/>
+      <c r="D63" s="20">
         <f t="shared" ref="D63:D64" si="6">COUNTIF($L$7:$L$55,$A63)</f>
         <v>14</v>
       </c>
-      <c r="E63" s="22"/>
+      <c r="E63" s="21"/>
       <c r="F63" s="9"/>
     </row>
     <row r="64" spans="1:270" ht="15">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="21">
+      <c r="B64" s="20">
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="C64" s="22"/>
-      <c r="D64" s="21">
+      <c r="C64" s="21"/>
+      <c r="D64" s="20">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="E64" s="22"/>
+      <c r="E64" s="21"/>
       <c r="F64" s="9"/>
     </row>
   </sheetData>
@@ -7149,7 +7182,6 @@
     <mergeCell ref="D63:E63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>